<commit_message>
Updating the sheet with mesh names
</commit_message>
<xml_diff>
--- a/Final_dataset for mesh cutting.xlsx
+++ b/Final_dataset for mesh cutting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni_Projects\3DMeshes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni_Projects\3DMeshes\Preprocessing3DMeshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A95DDAC-BE4F-40D7-BA5E-7CD93E00B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D659EEF1-19F8-487E-BECC-3AA7FF8AC9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94EF91F0-C53B-4769-8A56-5B61630E45BA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{94EF91F0-C53B-4769-8A56-5B61630E45BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>File Name</t>
   </si>
@@ -307,6 +307,36 @@
   </si>
   <si>
     <t>mesh_in_010</t>
+  </si>
+  <si>
+    <t>mesh_in_011</t>
+  </si>
+  <si>
+    <t>mesh_in_012</t>
+  </si>
+  <si>
+    <t>mesh_in_013</t>
+  </si>
+  <si>
+    <t>mesh_in_014</t>
+  </si>
+  <si>
+    <t>mesh_in_015</t>
+  </si>
+  <si>
+    <t>mesh_in_016</t>
+  </si>
+  <si>
+    <t>mesh_in_017</t>
+  </si>
+  <si>
+    <t>mesh_in_018</t>
+  </si>
+  <si>
+    <t>mesh_in_019</t>
+  </si>
+  <si>
+    <t>mesh_in_020</t>
   </si>
 </sst>
 </file>
@@ -344,7 +374,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +423,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -654,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -761,34 +797,37 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1108,7 +1147,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,8 +1188,11 @@
       <c r="D2" s="33">
         <v>10901</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="44" t="s">
         <v>82</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1166,7 +1208,10 @@
       <c r="D3" s="34">
         <v>18516</v>
       </c>
-      <c r="E3" s="36"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="46" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
@@ -1181,7 +1226,10 @@
       <c r="D4" s="35">
         <v>20271</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="46" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
@@ -1196,7 +1244,10 @@
       <c r="D5" s="34">
         <v>39848</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="46" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
@@ -1211,7 +1262,10 @@
       <c r="D6" s="34">
         <v>44234</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="46" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
@@ -1226,7 +1280,10 @@
       <c r="D7" s="34">
         <v>48864</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="46" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
@@ -1241,7 +1298,10 @@
       <c r="D8" s="34">
         <v>48864</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="46" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
@@ -1256,7 +1316,10 @@
       <c r="D9" s="34">
         <v>49147</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="46" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
@@ -1271,28 +1334,34 @@
       <c r="D10" s="34">
         <v>49618</v>
       </c>
-      <c r="E10" s="36"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="46" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="37">
         <v>27626</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>55292</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="43">
+      <c r="A12" s="41">
         <v>11</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="42" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="11">
@@ -1301,18 +1370,18 @@
       <c r="D12" s="11">
         <v>55292</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="39" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="43">
+      <c r="A13" s="41">
         <v>12</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="42" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="11">
@@ -1321,16 +1390,16 @@
       <c r="D13" s="11">
         <v>57216</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="42" t="s">
+      <c r="E13" s="44"/>
+      <c r="F13" s="40" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="43">
+      <c r="A14" s="41">
         <v>13</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="42" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="11">
@@ -1339,16 +1408,16 @@
       <c r="D14" s="11">
         <v>59372</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="41" t="s">
+      <c r="E14" s="44"/>
+      <c r="F14" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="43">
+      <c r="A15" s="41">
         <v>14</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="14">
@@ -1357,16 +1426,16 @@
       <c r="D15" s="11">
         <v>59740</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="41" t="s">
+      <c r="E15" s="44"/>
+      <c r="F15" s="39" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="43">
+      <c r="A16" s="41">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="42" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="11">
@@ -1375,16 +1444,16 @@
       <c r="D16" s="11">
         <v>60274</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="41" t="s">
+      <c r="E16" s="44"/>
+      <c r="F16" s="39" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="43">
+      <c r="A17" s="41">
         <v>16</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="11">
@@ -1393,16 +1462,16 @@
       <c r="D17" s="11">
         <v>64822</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="41" t="s">
+      <c r="E17" s="44"/>
+      <c r="F17" s="39" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="43">
+      <c r="A18" s="41">
         <v>17</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="42" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="11">
@@ -1411,16 +1480,16 @@
       <c r="D18" s="11">
         <v>64947</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="41" t="s">
+      <c r="E18" s="44"/>
+      <c r="F18" s="39" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="43">
+      <c r="A19" s="41">
         <v>18</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="42" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="11">
@@ -1429,16 +1498,16 @@
       <c r="D19" s="11">
         <v>65419</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="41" t="s">
+      <c r="E19" s="44"/>
+      <c r="F19" s="39" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="43">
+      <c r="A20" s="41">
         <v>19</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="42" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="11">
@@ -1447,16 +1516,16 @@
       <c r="D20" s="11">
         <v>73834</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="44"/>
+      <c r="F20" s="39" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="45">
+      <c r="A21" s="43">
         <v>20</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="42" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="11">
@@ -1465,8 +1534,8 @@
       <c r="D21" s="11">
         <v>74678</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="41" t="s">
+      <c r="E21" s="44"/>
+      <c r="F21" s="39" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding new pre-processed meshes
</commit_message>
<xml_diff>
--- a/Final_dataset for mesh cutting.xlsx
+++ b/Final_dataset for mesh cutting.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni_Projects\3DMeshes\Preprocessing3DMeshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D659EEF1-19F8-487E-BECC-3AA7FF8AC9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C25E461-C28A-4B37-B6E7-A085A1F6F41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{94EF91F0-C53B-4769-8A56-5B61630E45BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94EF91F0-C53B-4769-8A56-5B61630E45BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>File Name</t>
   </si>
@@ -273,12 +274,6 @@
     <t># Faces</t>
   </si>
   <si>
-    <t>LK</t>
-  </si>
-  <si>
-    <t>VS</t>
-  </si>
-  <si>
     <t>mesh_in_001</t>
   </si>
   <si>
@@ -337,13 +332,55 @@
   </si>
   <si>
     <t>mesh_in_020</t>
+  </si>
+  <si>
+    <t>5000 - 10000</t>
+  </si>
+  <si>
+    <t>10000 - 15000</t>
+  </si>
+  <si>
+    <t>15000 - 20000</t>
+  </si>
+  <si>
+    <t>20000 - 25000</t>
+  </si>
+  <si>
+    <t>25000 - 30000</t>
+  </si>
+  <si>
+    <t>30000 - 35000</t>
+  </si>
+  <si>
+    <t>35000 - 40000</t>
+  </si>
+  <si>
+    <t>10000 - 20000</t>
+  </si>
+  <si>
+    <t>20000 - 30000</t>
+  </si>
+  <si>
+    <t>30000 - 40000</t>
+  </si>
+  <si>
+    <t>40000 - 50000</t>
+  </si>
+  <si>
+    <t>50000 - 60000</t>
+  </si>
+  <si>
+    <t>60000 - 70000</t>
+  </si>
+  <si>
+    <t>70000 - 80000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +409,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -690,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -821,14 +864,23 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,6 +897,2167 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>Distribution of vertices</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$G$2:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5000 - 10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000 - 15000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000 - 20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000 - 25000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000 - 30000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000 - 35000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000 - 40000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25FA-4B88-A3E7-7254FB0BFE5B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="20"/>
+        <c:overlap val="-7"/>
+        <c:axId val="562787280"/>
+        <c:axId val="482051408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="562787280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-DE"/>
+                  <a:t>Number of vertices</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="482051408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="482051408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-DE"/>
+                  <a:t>Number of meshes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562787280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="480000"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>Distribution of faces</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$5:$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10000 - 20000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000 - 30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000 - 40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40000 - 50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000 - 60000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000 - 70000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000 - 80000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3DDC-47B9-85D4-00972FEF9D5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="14"/>
+        <c:overlap val="-27"/>
+        <c:axId val="473783544"/>
+        <c:axId val="473785464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="473783544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-DE"/>
+                  <a:t>Number of faces</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473785464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="473785464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-DE"/>
+                  <a:t>Number of meshes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473783544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600">
+          <a:latin typeface="Lucida Sans" panose="020B0602030504020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E975D9C8-98BA-4A3F-B6D8-EC9AEEEBE7D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>137159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CE95AF-3D71-415D-837A-B5EBD69EE203}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1144,24 +3357,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE29921-A217-4DB6-B26F-2711B732DA78}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="43.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -1175,7 +3389,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1189,13 +3403,16 @@
         <v>10901</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1208,12 +3425,17 @@
       <c r="D3" s="34">
         <v>18516</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1226,12 +3448,17 @@
       <c r="D4" s="35">
         <v>20271</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1244,12 +3471,17 @@
       <c r="D5" s="34">
         <v>39848</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1262,12 +3494,17 @@
       <c r="D6" s="34">
         <v>44234</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1280,12 +3517,17 @@
       <c r="D7" s="34">
         <v>48864</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1298,12 +3540,17 @@
       <c r="D8" s="34">
         <v>48864</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1316,12 +3563,11 @@
       <c r="D9" s="34">
         <v>49147</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1334,12 +3580,11 @@
       <c r="D10" s="34">
         <v>49618</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1352,12 +3597,11 @@
       <c r="D11" s="38">
         <v>55292</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
         <v>11</v>
       </c>
@@ -1370,14 +3614,11 @@
       <c r="D12" s="11">
         <v>55292</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="41">
         <v>12</v>
       </c>
@@ -1390,12 +3631,11 @@
       <c r="D13" s="11">
         <v>57216</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="41">
         <v>13</v>
       </c>
@@ -1408,12 +3648,11 @@
       <c r="D14" s="11">
         <v>59372</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
         <v>14</v>
       </c>
@@ -1426,12 +3665,11 @@
       <c r="D15" s="11">
         <v>59740</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="41">
         <v>15</v>
       </c>
@@ -1444,12 +3682,11 @@
       <c r="D16" s="11">
         <v>60274</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="41">
         <v>16</v>
       </c>
@@ -1462,12 +3699,11 @@
       <c r="D17" s="11">
         <v>64822</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="41">
         <v>17</v>
       </c>
@@ -1480,12 +3716,11 @@
       <c r="D18" s="11">
         <v>64947</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="41">
         <v>18</v>
       </c>
@@ -1498,12 +3733,11 @@
       <c r="D19" s="11">
         <v>65419</v>
       </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="41">
         <v>19</v>
       </c>
@@ -1516,12 +3750,11 @@
       <c r="D20" s="11">
         <v>73834</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="43">
         <v>20</v>
       </c>
@@ -1534,12 +3767,11 @@
       <c r="D21" s="11">
         <v>74678</v>
       </c>
-      <c r="E21" s="44"/>
-      <c r="F21" s="39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -1553,7 +3785,7 @@
         <v>78963</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -1567,7 +3799,7 @@
         <v>83888</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -1581,7 +3813,7 @@
         <v>86530</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -1595,7 +3827,7 @@
         <v>86530</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -1609,7 +3841,7 @@
         <v>88230</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -1623,7 +3855,7 @@
         <v>88606</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -1637,7 +3869,7 @@
         <v>95464</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -1651,7 +3883,7 @@
         <v>101874</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -1665,7 +3897,7 @@
         <v>104042</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -1679,7 +3911,7 @@
         <v>106586</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -2352,14 +4584,180 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D1047654">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E79">
     <sortCondition ref="C1:C1047654"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="E2:E11"/>
-    <mergeCell ref="E12:E21"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52A6FAD-0F01-41D5-ABF3-66B927F338BF}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="45">
+        <v>10901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A3" s="46">
+        <v>18516</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A4" s="47">
+        <v>20271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" s="46">
+        <v>39848</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="46">
+        <v>44234</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="46">
+        <v>48864</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="46">
+        <v>48864</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="46">
+        <v>49147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="46">
+        <v>49618</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="48">
+        <v>55292</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="49">
+        <v>55292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="49">
+        <v>57216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" s="49">
+        <v>59372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A15" s="49">
+        <v>59740</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A16" s="49">
+        <v>60274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="49">
+        <v>64822</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A18" s="49">
+        <v>64947</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A19" s="49">
+        <v>65419</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A20" s="49">
+        <v>73834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A21" s="49">
+        <v>74678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding notebook for IOU calculation
</commit_message>
<xml_diff>
--- a/Final_dataset for mesh cutting.xlsx
+++ b/Final_dataset for mesh cutting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni_Projects\3DMeshes\Preprocessing3DMeshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C25E461-C28A-4B37-B6E7-A085A1F6F41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71911941-1972-4A29-94F0-633F08A4B80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94EF91F0-C53B-4769-8A56-5B61630E45BA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{94EF91F0-C53B-4769-8A56-5B61630E45BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t>File Name</t>
   </si>
@@ -334,46 +334,70 @@
     <t>mesh_in_020</t>
   </si>
   <si>
-    <t>5000 - 10000</t>
-  </si>
-  <si>
-    <t>10000 - 15000</t>
-  </si>
-  <si>
-    <t>15000 - 20000</t>
-  </si>
-  <si>
-    <t>20000 - 25000</t>
-  </si>
-  <si>
-    <t>25000 - 30000</t>
-  </si>
-  <si>
-    <t>30000 - 35000</t>
-  </si>
-  <si>
-    <t>35000 - 40000</t>
-  </si>
-  <si>
-    <t>10000 - 20000</t>
-  </si>
-  <si>
-    <t>20000 - 30000</t>
-  </si>
-  <si>
-    <t>30000 - 40000</t>
-  </si>
-  <si>
-    <t>40000 - 50000</t>
-  </si>
-  <si>
-    <t>50000 - 60000</t>
-  </si>
-  <si>
-    <t>60000 - 70000</t>
-  </si>
-  <si>
-    <t>70000 - 80000</t>
+    <t>5000-20000</t>
+  </si>
+  <si>
+    <t>20000-35000</t>
+  </si>
+  <si>
+    <t>35000-50000</t>
+  </si>
+  <si>
+    <t>50000-65000</t>
+  </si>
+  <si>
+    <t>65000-80000</t>
+  </si>
+  <si>
+    <t>80000-95000</t>
+  </si>
+  <si>
+    <t>95000-110000</t>
+  </si>
+  <si>
+    <t>110000-125000</t>
+  </si>
+  <si>
+    <t>125000-140000</t>
+  </si>
+  <si>
+    <t>140000-155000</t>
+  </si>
+  <si>
+    <t>155000-170000</t>
+  </si>
+  <si>
+    <t>10000-40000</t>
+  </si>
+  <si>
+    <t>40000-70000</t>
+  </si>
+  <si>
+    <t>70000-100000</t>
+  </si>
+  <si>
+    <t>100000-130000</t>
+  </si>
+  <si>
+    <t>130000-160000</t>
+  </si>
+  <si>
+    <t>160000-190000</t>
+  </si>
+  <si>
+    <t>190000-220000</t>
+  </si>
+  <si>
+    <t>220000-250000</t>
+  </si>
+  <si>
+    <t>250000-280000</t>
+  </si>
+  <si>
+    <t>280000-310000</t>
+  </si>
+  <si>
+    <t>310000-340000</t>
   </si>
 </sst>
 </file>
@@ -1049,59 +1073,83 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$G$2:$G$8</c:f>
+              <c:f>Tabelle1!$G$2:$G$12</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5000 - 10000</c:v>
+                  <c:v>5000-20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10000 - 15000</c:v>
+                  <c:v>20000-35000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15000 - 20000</c:v>
+                  <c:v>35000-50000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20000 - 25000</c:v>
+                  <c:v>50000-65000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25000 - 30000</c:v>
+                  <c:v>65000-80000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30000 - 35000</c:v>
+                  <c:v>80000-95000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35000 - 40000</c:v>
+                  <c:v>95000-110000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110000-125000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>125000-140000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140000-155000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155000-170000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$2:$H$8</c:f>
+              <c:f>Tabelle1!$H$2:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1211,7 +1259,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1542,59 +1590,83 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$5:$D$11</c:f>
+              <c:f>Sheet1!$D$5:$D$15</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>10000 - 20000</c:v>
+                  <c:v>10000-40000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20000 - 30000</c:v>
+                  <c:v>40000-70000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30000 - 40000</c:v>
+                  <c:v>70000-100000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40000 - 50000</c:v>
+                  <c:v>100000-130000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000 - 60000</c:v>
+                  <c:v>130000-160000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60000 - 70000</c:v>
+                  <c:v>160000-190000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70000 - 80000</c:v>
+                  <c:v>190000-220000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>220000-250000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250000-280000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280000-310000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>310000-340000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$11</c:f>
+              <c:f>Sheet1!$E$5:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,7 +1776,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2983,15 +3055,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>135890</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>206374</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>16510</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3023,16 +3095,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>137159</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>68579</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3359,8 +3431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE29921-A217-4DB6-B26F-2711B732DA78}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3409,7 +3481,7 @@
         <v>102</v>
       </c>
       <c r="H2" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -3432,7 +3504,7 @@
         <v>103</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3455,7 +3527,7 @@
         <v>104</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3478,7 +3550,7 @@
         <v>105</v>
       </c>
       <c r="H5" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3501,7 +3573,7 @@
         <v>106</v>
       </c>
       <c r="H6" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3524,7 +3596,7 @@
         <v>107</v>
       </c>
       <c r="H7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3547,7 +3619,7 @@
         <v>108</v>
       </c>
       <c r="H8" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -3566,6 +3638,12 @@
       <c r="E9" s="44" t="s">
         <v>99</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
@@ -3583,6 +3661,12 @@
       <c r="E10" s="44" t="s">
         <v>100</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
@@ -3600,6 +3684,12 @@
       <c r="E11" s="44" t="s">
         <v>101</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
@@ -3616,6 +3706,12 @@
       </c>
       <c r="E12" s="39" t="s">
         <v>82</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -4598,14 +4694,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52A6FAD-0F01-41D5-ABF3-66B927F338BF}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4633,10 +4729,10 @@
         <v>39848</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4644,10 +4740,10 @@
         <v>44234</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4655,10 +4751,10 @@
         <v>48864</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4666,10 +4762,10 @@
         <v>48864</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4677,10 +4773,10 @@
         <v>49147</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4688,10 +4784,10 @@
         <v>49618</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4699,30 +4795,54 @@
         <v>55292</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="49">
         <v>55292</v>
       </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="49">
         <v>57216</v>
       </c>
+      <c r="D13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="49">
         <v>59372</v>
       </c>
+      <c r="D14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="49">
         <v>59740</v>
+      </c>
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">

</xml_diff>